<commit_message>
pidan: tune mc nc kc and tune prefetch but only get 83% peak performance
</commit_message>
<xml_diff>
--- a/testing/performance/perfData.xlsx
+++ b/testing/performance/perfData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pidan/guoke/研二上/工作/gemm_opt/pidan_cpu_gemm_opt/testing/performance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E00712-0ED8-7D4F-B701-C4D3B8A6AE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC83BF9-C67D-6A41-AF8D-FCEDC4D2AB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9880" yWindow="1740" windowWidth="28240" windowHeight="17440" xr2:uid="{447EC727-2300-CA43-BCC7-E641CF6323F0}"/>
+    <workbookView xWindow="6380" yWindow="4900" windowWidth="28240" windowHeight="17440" xr2:uid="{447EC727-2300-CA43-BCC7-E641CF6323F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>openblas</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,6 +68,18 @@
   </si>
   <si>
     <t>62(81.5%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pidan tune mc nc kc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>63.31(83%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pidan add prefetch in pack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -434,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077025A6-C14D-6A42-9E07-A1A1622C1056}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -446,11 +459,12 @@
     <col min="2" max="2" width="17.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
     <col min="4" max="4" width="19.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="6" width="26.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -466,8 +480,14 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>4128</v>
       </c>
@@ -482,6 +502,12 @@
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pidan: test to get datas to write summary
</commit_message>
<xml_diff>
--- a/testing/performance/perfData.xlsx
+++ b/testing/performance/perfData.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pidan/guoke/研二上/工作/gemm_opt/pidan_cpu_gemm_opt/testing/performance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC83BF9-C67D-6A41-AF8D-FCEDC4D2AB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBD2F0C-EF59-D148-8432-2C13B5C77E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="4900" windowWidth="28240" windowHeight="17440" xr2:uid="{447EC727-2300-CA43-BCC7-E641CF6323F0}"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="28240" windowHeight="17440" xr2:uid="{447EC727-2300-CA43-BCC7-E641CF6323F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>openblas</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,11 +74,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>63.31(83%)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pidan add prefetch in pack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>67(88%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>66(86%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65(85%)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -447,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077025A6-C14D-6A42-9E07-A1A1622C1056}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -481,7 +488,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>9</v>
@@ -507,7 +514,18 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>1152</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>